<commit_message>
Bug fixes and torn categories
Character polaroids and Category notes are now torn off when unavailable (non existent or just locked)
A random player now starts instead of always player 1
Added a hover effect to notes and polaroids
Fixed an issue where after every game you'd get the levelled up popup, even when not levelling up
Fixed an issue where the level popup says "LevelX" instead of "Level X"
Fixed an issue where if your first list wasn't the default list (somehow), it'd replace that list instead of creating a new one
Fixed an issue where you could press done even if you have to accuse
Fixed an issue where the connection note would sometimes be disabled
Removed Carnie out of the default list and replaced him with Bub
Bub now gets unlock by default instead of being locked at level 4
Slight optimisation in some scripts
Updated game version to 97
</commit_message>
<xml_diff>
--- a/Assets/Characters.xlsx
+++ b/Assets/Characters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joas\Unity\fnaf-guess-who\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2430EC2F-78D5-4FB0-8A77-C31FDD1313BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6A4981-5FF0-4D8A-82CF-34607D14221F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFDEBCCC-71C8-4C9A-803B-30C727DDBE09}"/>
   </bookViews>
@@ -1030,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DF9DEC-5089-403D-8BE4-09376149DA9A}">
   <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,21 +1845,21 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E57" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1873,7 +1873,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -1929,7 +1929,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -1943,21 +1943,21 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>11</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E64" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -1999,21 +1999,21 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="B68">
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="E68" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2069,77 +2069,77 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E73" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>128</v>
+        <v>70</v>
       </c>
       <c r="B74">
         <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="E74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B75">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E75" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="B76">
         <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E76" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="B77">
         <v>3</v>
       </c>
       <c r="C77" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E77" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B78">
         <v>3</v>
@@ -2148,54 +2148,54 @@
         <v>149</v>
       </c>
       <c r="E78" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="B79">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E79" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="B80">
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E80" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="B81">
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E81" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B83">
         <v>4</v>
@@ -2223,7 +2223,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B84">
         <v>4</v>
@@ -2237,7 +2237,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B85">
         <v>4</v>
@@ -2251,16 +2251,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="B86">
         <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="E86" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>